<commit_message>
TPO33 Con University's policies regarding dorm rooms
</commit_message>
<xml_diff>
--- a/TPO_Listening.xlsx
+++ b/TPO_Listening.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\imdan\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\codehub\TPO_shuati_Record\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71CDE8E3-8D4F-4E8D-BC14-2A69E3CED246}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB0E3231-C12F-4E5B-A7A6-4174098D19F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="22320" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>TPO</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -479,6 +479,10 @@
       </rPr>
       <t>-The classification of Creatures</t>
     </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>University's policies regarding dorm rooms</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -551,10 +555,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -842,13 +847,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F25" sqref="F25"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B39" sqref="B39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="36" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="42.88671875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="40.5546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="30" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="48" bestFit="1" customWidth="1"/>
@@ -1107,6 +1112,9 @@
       <c r="A39">
         <v>33</v>
       </c>
+      <c r="B39" s="3" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40">
@@ -1286,6 +1294,6 @@
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" copies="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>